<commit_message>
stash species with no eBird data
</commit_message>
<xml_diff>
--- a/old/pending/pending - atlas_list.xlsx
+++ b/old/pending/pending - atlas_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\old\stashed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\old\pending\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3A0E0FC-CB23-4F0B-8102-8464DA2FC51F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E168692-683C-4C76-B141-8BB76FDCAB35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{5131612B-3B01-4B1D-86DE-442CCA8B90C0}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>Anser sp. (Domestic type)</t>
   </si>
@@ -66,6 +66,42 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>Anous albivitta</t>
+  </si>
+  <si>
+    <t>Grey Ternlet</t>
+  </si>
+  <si>
+    <t>Not threatened; Marine; Not migratory</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Aplonis metallica</t>
+  </si>
+  <si>
+    <t>Metallic Starling</t>
+  </si>
+  <si>
+    <t>Charadrius veredus</t>
+  </si>
+  <si>
+    <t>Oriental Plover</t>
+  </si>
+  <si>
+    <t>Not threatened; Marine; Migratory (Bonn, CAMBA, JAMBA, ROKAMBA)</t>
+  </si>
+  <si>
+    <t>Pachyptila salvini</t>
+  </si>
+  <si>
+    <t>Salvin's Prion</t>
   </si>
 </sst>
 </file>
@@ -421,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58730256-3AA8-42A7-865E-01E0A5630275}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +553,170 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>28322</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>2005</v>
+      </c>
+      <c r="J3">
+        <v>1700</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6321</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>2005</v>
+      </c>
+      <c r="J4">
+        <v>1700</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5706</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2005</v>
+      </c>
+      <c r="J5">
+        <v>1700</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6716</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2005</v>
+      </c>
+      <c r="J6">
+        <v>1700</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6">
+        <v>544</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove old pending documents
</commit_message>
<xml_diff>
--- a/old/pending/pending - atlas_list.xlsx
+++ b/old/pending/pending - atlas_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\old\pending\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E168692-683C-4C76-B141-8BB76FDCAB35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BD8544-05D4-4B29-86D0-E70277E607AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{5131612B-3B01-4B1D-86DE-442CCA8B90C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5131612B-3B01-4B1D-86DE-442CCA8B90C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Anser sp. (Domestic type)</t>
   </si>
@@ -66,42 +66,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>Anous albivitta</t>
-  </si>
-  <si>
-    <t>Grey Ternlet</t>
-  </si>
-  <si>
-    <t>Not threatened; Marine; Not migratory</t>
-  </si>
-  <si>
-    <t>both</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Aplonis metallica</t>
-  </si>
-  <si>
-    <t>Metallic Starling</t>
-  </si>
-  <si>
-    <t>Charadrius veredus</t>
-  </si>
-  <si>
-    <t>Oriental Plover</t>
-  </si>
-  <si>
-    <t>Not threatened; Marine; Migratory (Bonn, CAMBA, JAMBA, ROKAMBA)</t>
-  </si>
-  <si>
-    <t>Pachyptila salvini</t>
-  </si>
-  <si>
-    <t>Salvin's Prion</t>
   </si>
 </sst>
 </file>
@@ -457,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58730256-3AA8-42A7-865E-01E0A5630275}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,170 +517,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>28322</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>2005</v>
-      </c>
-      <c r="J3">
-        <v>1700</v>
-      </c>
-      <c r="K3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3">
-        <v>1935</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6321</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>2005</v>
-      </c>
-      <c r="J4">
-        <v>1700</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5706</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>2005</v>
-      </c>
-      <c r="J5">
-        <v>1700</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N5" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6716</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <v>2005</v>
-      </c>
-      <c r="J6">
-        <v>1700</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6">
-        <v>544</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>